<commit_message>
More work on PT2, update project plan
</commit_message>
<xml_diff>
--- a/Documentation/Preliminary Release/Updated Project Plan (Gantt chart).xlsx
+++ b/Documentation/Preliminary Release/Updated Project Plan (Gantt chart).xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\studenthome.cis.strath.ac.uk\homes\system\Windows\Desktop\Preliminary Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\system\Windows\Desktop\CS308\Gizmoball - MW1\Documentation\Preliminary Release\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -428,6 +428,34 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">Prototype 3 Implementation (Load Board) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Greig Cairns)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prototype 4 Implementation (Flipper)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (Thomas Mclaughlin)</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t>Prototype 2 Implementation (Collisions)</t>
     </r>
     <r>
@@ -437,35 +465,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> (David T. Pocock/Greig Cairns/Tomas Šukevičius)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Prototype 3 Implementation (Load Board) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>(Greig Cairns)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Prototype 4 Implementation (Flipper)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (Thomas Mclaughlin/Chris Reilly)</t>
+      <t xml:space="preserve"> (David T. Pocock)</t>
     </r>
   </si>
 </sst>
@@ -1860,7 +1860,7 @@
   <dimension ref="B1:EQ34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2416,7 +2416,7 @@
     </row>
     <row r="25" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C25" s="32">
         <v>3</v>
@@ -2437,7 +2437,7 @@
     </row>
     <row r="26" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C26" s="32">
         <v>5</v>
@@ -2458,7 +2458,7 @@
     </row>
     <row r="27" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C27" s="32">
         <v>3</v>

</xml_diff>